<commit_message>
menu selected and postage settings
</commit_message>
<xml_diff>
--- a/public/export.xlsx
+++ b/public/export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>Id</t>
   </si>
@@ -74,51 +74,43 @@
     <t>Updated</t>
   </si>
   <si>
-    <t xml:space="preserve">Bridge of Song, the :  For Iowa's Singing
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small area of discoloration on front. No other defects.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21522
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very Good
-</t>
-  </si>
-  <si>
-    <t>{"Author":"Exner, Max V.\r\n","Category":"Music\r\n","Publisher":"Cooperative Recreation Service\r\n","DatePublished":"1957\r\n","Binding":"Softcover\r\n","Keywords":"4-H Club ;\r\n","Weight":"0.3\r\n","4":"4\r\n","1":"1\r\n","BO":"BO\r\n","S":"S"}</t>
+    <t>American Country Churches</t>
+  </si>
+  <si>
+    <t>beautiful publication.</t>
+  </si>
+  <si>
+    <t>Used- Good</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>cat20200529_121634.png</t>
+  </si>
+  <si>
+    <t>{"Author":"Morgan, William; Illustrated by Radek Kurzaj\r\n","Category":"Architecture\r\n","Publisher":"Harry N. Abrams\r\n","DatePublished":"2004\r\n","Edition":"Second Printing\r\n","Binding":"Hardcover\r\n","Keywords":"Religion &amp; Spirituality ;\r\n","Weight":"3.3\r\n","4":"4\r\n","1":"1\r\n","BO":"BO\r\n","S":"S"}</t>
   </si>
   <si>
     <t>2020-05-05 18:10:58</t>
   </si>
   <si>
-    <t>American Country Churches</t>
-  </si>
-  <si>
-    <t>beautiful publication.</t>
-  </si>
-  <si>
-    <t>Used- Good</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>cat20200529_121634.png</t>
-  </si>
-  <si>
-    <t>{"Author":"Morgan, William; Illustrated by Radek Kurzaj\r\n","Category":"Architecture\r\n","Publisher":"Harry N. Abrams\r\n","DatePublished":"2004\r\n","Edition":"Second Printing\r\n","Binding":"Hardcover\r\n","Keywords":"Religion &amp; Spirituality ;\r\n","Weight":"3.3\r\n","4":"4\r\n","1":"1\r\n","BO":"BO\r\n","S":"S"}</t>
-  </si>
-  <si>
     <t>2020-05-29 12:18:21</t>
+  </si>
+  <si>
+    <t>Evans, Edie</t>
+  </si>
+  <si>
+    <t>33500995071</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>{"Seller":83,"Title":"I Love You, Mommy (Little Golden Book)","Illustrator":null,"BookSize":null,"JacketCondition":null,"Binding":"Hardcover","BookType":null,"Publisher":"Golden Books","PublishPlace":null,"PublishDate":"Dec-99","Edition":null,"Inscription":null,"Description":null,"Image":null,"Category1":"Children's General","Category2":null,"Category3":null,"Category4":null,"Category5":null,"Keyword1":null,"Keyword2":null,"Keyword3":null,"Keyword4":null,"Keyword5":null,"Keyword6":null,"Keyword7":null,"Keyword8":null,"Keyword9":null,"Weight":null,"FeaturedItem":null}</t>
+  </si>
+  <si>
+    <t>2020-06-03 09:38:38</t>
   </si>
 </sst>
 </file>
@@ -526,7 +518,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>
@@ -534,33 +526,39 @@
       <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2">
+        <v>21503</v>
+      </c>
+      <c r="E2">
+        <v>345</v>
+      </c>
+      <c r="F2">
+        <v>11.0</v>
+      </c>
+      <c r="G2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2">
-        <v>5.0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>23</v>
-      </c>
       <c r="H2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2"/>
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
       <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2"/>
-      <c r="N2"/>
+        <v>123</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2">
+        <v>2</v>
+      </c>
       <c r="O2">
         <v>0</v>
       </c>
@@ -574,52 +572,42 @@
         <v>25</v>
       </c>
       <c r="S2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
         <v>27</v>
       </c>
-      <c r="D3">
-        <v>21503</v>
-      </c>
-      <c r="E3">
-        <v>345</v>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3" t="s">
+        <v>28</v>
       </c>
       <c r="F3">
-        <v>11.0</v>
+        <v>80.0</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K3"/>
       <c r="L3">
-        <v>123</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3">
-        <v>2</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="M3"/>
+      <c r="N3"/>
       <c r="O3">
         <v>0</v>
       </c>
@@ -627,13 +615,13 @@
         <v>24</v>
       </c>
       <c r="Q3" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" t="s">
         <v>31</v>
       </c>
-      <c r="R3" t="s">
-        <v>25</v>
-      </c>
       <c r="S3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>